<commit_message>
Preparando o projeto para trabalhar com vários sites diferentes.
</commit_message>
<xml_diff>
--- a/Python/ProjetoIptvManterLinkUsuarioAtualizado/Clientes.xlsx
+++ b/Python/ProjetoIptvManterLinkUsuarioAtualizado/Clientes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjetosLuiz\Projects\Python\ProjetoIptvManterLinkUsuarioAtualizado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7593400-47A2-4935-A128-632FC7D0F75F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C80F5AB-BB6C-4492-B93B-91A30BF86683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3672" yWindow="2232" windowWidth="17280" windowHeight="8928" xr2:uid="{7F01D1A6-D05C-4EE5-AEA0-5513D690E58D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7F01D1A6-D05C-4EE5-AEA0-5513D690E58D}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
   <si>
     <t>Servidor</t>
   </si>
@@ -84,6 +84,36 @@
   </si>
   <si>
     <t>Cliente IPTV 86</t>
+  </si>
+  <si>
+    <t>Cliente IPTV 209 Uniplay</t>
+  </si>
+  <si>
+    <t>d4:9d:c0:c7:7c:9e</t>
+  </si>
+  <si>
+    <t>UNIPLAY</t>
+  </si>
+  <si>
+    <t>34:f1:00:cd:6a:ca</t>
+  </si>
+  <si>
+    <t>Heloiza TVS Cliente IPTV Tia Vinícius</t>
+  </si>
+  <si>
+    <t>e9:f5:d8:02:59:4a</t>
+  </si>
+  <si>
+    <t>Site ativação</t>
+  </si>
+  <si>
+    <t>iboplayer.com</t>
+  </si>
+  <si>
+    <t>iboplayer.pro</t>
+  </si>
+  <si>
+    <t>Cliente IPTV 215</t>
   </si>
 </sst>
 </file>
@@ -107,12 +137,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -127,9 +163,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,15 +504,16 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -491,6 +529,9 @@
       <c r="D1" t="s">
         <v>0</v>
       </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -505,6 +546,9 @@
       <c r="D2" t="s">
         <v>2</v>
       </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -519,6 +563,9 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -533,6 +580,9 @@
       <c r="D4" t="s">
         <v>7</v>
       </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -547,6 +597,10 @@
       <c r="D5" t="s">
         <v>7</v>
       </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -560,6 +614,60 @@
       </c>
       <c r="D6" t="s">
         <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7">
+        <v>333720</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8">
+        <v>183507</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="2">
+        <v>701063</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>